<commit_message>
Osprey Admin ProDeal Testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF91D91B-305B-4C53-8C10-C0D2CB16813F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B920716-312D-4BA3-89C3-26C846691877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>DataSet</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>AccountDetails</t>
+  </si>
+  <si>
+    <t>sbingi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Auislzkuakm03!</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>ProDeal</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>AssociationEmail</t>
+  </si>
+  <si>
+    <t>skasarla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>ProDealForm</t>
+  </si>
+  <si>
+    <t>nsada@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Qa testing the prodeal form</t>
   </si>
 </sst>
 </file>
@@ -46,14 +121,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,12 +160,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -373,79 +449,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.88671875" customWidth="1"/>
-    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -462,27 +563,70 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="D3" s="2"/>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4">
+        <v>976</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B19371E4-28DB-4D87-83B1-38BC504CA804}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{EA7030D4-0A74-4ACA-AF4C-FF1B10BB8EBD}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{D97F1CA6-F7D4-49A4-82F4-F7CD38291CF4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Osprey Admin CM & CrtPricerule and catlogPrice rule Code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B920716-312D-4BA3-89C3-26C846691877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{8B920716-312D-4BA3-89C3-26C846691877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34A31D3-D576-460F-9305-E4410BB91684}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="10275" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
+    <sheet name="Category" sheetId="2" r:id="rId2"/>
+    <sheet name="CartRulePrice" sheetId="3" r:id="rId3"/>
+    <sheet name="CatalogPricerule" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="223">
   <si>
     <t>DataSet</t>
   </si>
@@ -98,13 +101,604 @@
   </si>
   <si>
     <t>Qa testing the prodeal form</t>
+  </si>
+  <si>
+    <t>RootCategory</t>
+  </si>
+  <si>
+    <t>NewMaincategory</t>
+  </si>
+  <si>
+    <t>Newcategory</t>
+  </si>
+  <si>
+    <t>Newsubcategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DefaultCategory </t>
+  </si>
+  <si>
+    <t>TestCategory</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Updatesubcategory</t>
+  </si>
+  <si>
+    <t>cache</t>
+  </si>
+  <si>
+    <t>vnarra@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>mudhiraj@168</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Osprey_EU</t>
+  </si>
+  <si>
+    <t>TestRootCategory</t>
+  </si>
+  <si>
+    <t>Test Category2</t>
+  </si>
+  <si>
+    <t>New Category</t>
+  </si>
+  <si>
+    <t>Test Subcategory</t>
+  </si>
+  <si>
+    <t>Default Category (ID: 2) (5104)</t>
+  </si>
+  <si>
+    <t>Test Category (ID: 308) (5104)</t>
+  </si>
+  <si>
+    <t>https://mcloud-emea-staging.hele.digital</t>
+  </si>
+  <si>
+    <t>Magentocache</t>
+  </si>
+  <si>
+    <t>Flush Magento Cache</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Discount Amount</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>RuleName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Coupon</t>
+  </si>
+  <si>
+    <t>FinanceCategory</t>
+  </si>
+  <si>
+    <t>Coupon Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uses per Coupon</t>
+  </si>
+  <si>
+    <t>Uses per Customer</t>
+  </si>
+  <si>
+    <t>QtyProduct</t>
+  </si>
+  <si>
+    <t>streetaddress</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>SKUNumber</t>
+  </si>
+  <si>
+    <t>ExpMonth</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>SegmentName</t>
+  </si>
+  <si>
+    <t>taxclass</t>
+  </si>
+  <si>
+    <t>ApplyTo</t>
+  </si>
+  <si>
+    <t>AssignedStatus</t>
+  </si>
+  <si>
+    <t>customergroupname</t>
+  </si>
+  <si>
+    <t>Updatecustomergroupname</t>
+  </si>
+  <si>
+    <t>Adminsuccessmesaage</t>
+  </si>
+  <si>
+    <t>errormessage</t>
+  </si>
+  <si>
+    <t>Tiletext</t>
+  </si>
+  <si>
+    <t>textbutton</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>CategorySelect</t>
+  </si>
+  <si>
+    <t>productnames</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>VideoURL</t>
+  </si>
+  <si>
+    <t>CardTitle</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Buttontext</t>
+  </si>
+  <si>
+    <t>Buttontype</t>
+  </si>
+  <si>
+    <t>ButtonLinknavigation</t>
+  </si>
+  <si>
+    <t>ButtonlinkURL</t>
+  </si>
+  <si>
+    <t>Buttonlinkcategory</t>
+  </si>
+  <si>
+    <t>Buttonlinkproduct</t>
+  </si>
+  <si>
+    <t>Buttonlinkpage</t>
+  </si>
+  <si>
+    <t>ActualCategorydisplay</t>
+  </si>
+  <si>
+    <t>Categorydisplay</t>
+  </si>
+  <si>
+    <t>No.ofproductsdisplay</t>
+  </si>
+  <si>
+    <t>productcategory</t>
+  </si>
+  <si>
+    <t>Editpagetitle</t>
+  </si>
+  <si>
+    <t>datacontenttype</t>
+  </si>
+  <si>
+    <t>Deletcomponent</t>
+  </si>
+  <si>
+    <t>headingtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description Type</t>
+  </si>
+  <si>
+    <t>alterantivetext</t>
+  </si>
+  <si>
+    <t>titleaatribute</t>
+  </si>
+  <si>
+    <t>Customergrouppagetitle</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>MYAccountlinks</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Welcome Email</t>
+  </si>
+  <si>
+    <t>Acceptdate</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>ordernumber</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Productname</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Backgroud position</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>pageTitle</t>
+  </si>
+  <si>
+    <t>prodURL</t>
+  </si>
+  <si>
+    <t>preprodURL</t>
+  </si>
+  <si>
+    <t>mobilelayout</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>TextColor</t>
+  </si>
+  <si>
+    <t>CTA Type</t>
+  </si>
+  <si>
+    <t>CTA Link</t>
+  </si>
+  <si>
+    <t>CTAText</t>
+  </si>
+  <si>
+    <t>CTAurl</t>
+  </si>
+  <si>
+    <t>categoryname</t>
+  </si>
+  <si>
+    <t>mrgtop</t>
+  </si>
+  <si>
+    <t>mrgright</t>
+  </si>
+  <si>
+    <t>mrgbottom</t>
+  </si>
+  <si>
+    <t>mrgleft</t>
+  </si>
+  <si>
+    <t>paddingtop</t>
+  </si>
+  <si>
+    <t>paddingright</t>
+  </si>
+  <si>
+    <t>paddingbottom</t>
+  </si>
+  <si>
+    <t>paddingleft</t>
+  </si>
+  <si>
+    <t>CSSclasses</t>
+  </si>
+  <si>
+    <t>SubTitle</t>
+  </si>
+  <si>
+    <t>ChooseCondition</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>SpecialPrice</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Stock Status</t>
+  </si>
+  <si>
+    <t>Updateprice</t>
+  </si>
+  <si>
+    <t>updateStock Status</t>
+  </si>
+  <si>
+    <t>qatesting.lotuswave@gmail.com</t>
+  </si>
+  <si>
+    <t>Fixed amount discount for whole cart</t>
+  </si>
+  <si>
+    <t>Osprey UK</t>
+  </si>
+  <si>
+    <t>QA Test 20</t>
+  </si>
+  <si>
+    <t>To apply the cart price</t>
+  </si>
+  <si>
+    <t>Specific Coupon</t>
+  </si>
+  <si>
+    <t>TRADE</t>
+  </si>
+  <si>
+    <t>LOTUSQA20</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>844 N Colony Rd</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>06492</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page </t>
+  </si>
+  <si>
+    <t>Home Page (Hydroflask)</t>
+  </si>
+  <si>
+    <t>https://emea-stage.hele.digital/</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>POCO® CARRYING CASE</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Addressbook</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>###############################################################################################################################################################################################################################################################</t>
+  </si>
+  <si>
+    <t>GroundShippingmethod</t>
+  </si>
+  <si>
+    <t>Standard Shipping - FedEx Ground (2-5 Business Days)</t>
+  </si>
+  <si>
+    <t>PaymentDetails</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>addproduct</t>
+  </si>
+  <si>
+    <t>Financecategory</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>EUCategory</t>
+  </si>
+  <si>
+    <t>EUsubcategory</t>
+  </si>
+  <si>
+    <t>Discard subsequent rules</t>
+  </si>
+  <si>
+    <t>Updateproductname</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>Instock</t>
+  </si>
+  <si>
+    <t>CustomerGroup</t>
+  </si>
+  <si>
+    <t>QtyPrice</t>
+  </si>
+  <si>
+    <t>QtyPrice1</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>QATEST product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 QATEST product </t>
+  </si>
+  <si>
+    <t>Catalogpricedetails</t>
+  </si>
+  <si>
+    <t>Qatestcatalogrule</t>
+  </si>
+  <si>
+    <t>5%offcatalogpricerule</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Test Category (5104)</t>
+  </si>
+  <si>
+    <t>Categoryselection</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Apply as percentage of original</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>AdvancedPricing</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>QATestProduct</t>
+  </si>
+  <si>
+    <t>Productupdate</t>
+  </si>
+  <si>
+    <t>10 QATEST product</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>searchproduct</t>
+  </si>
+  <si>
+    <t>Stockstatus</t>
+  </si>
+  <si>
+    <t>In Stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +722,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,7 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -168,6 +769,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -629,4 +1233,999 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1810791-6AFF-44EB-BA66-A2C45D322E0B}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{D4D25C80-01BA-4623-95CD-5DB20E2FFF79}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005B9DD-FA95-4DB7-BA01-87E095E7225F}">
+  <dimension ref="A1:DU9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:DU9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DN1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DO1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R2">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" t="s">
+        <v>15</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>170</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CE2" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CF2">
+        <v>9898989898</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>176</v>
+      </c>
+      <c r="DU3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" t="s">
+        <v>179</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
+        <v>161</v>
+      </c>
+      <c r="O5" t="s">
+        <v>170</v>
+      </c>
+      <c r="P5" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" t="s">
+        <v>173</v>
+      </c>
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T5" t="s">
+        <v>183</v>
+      </c>
+      <c r="U5" t="s">
+        <v>15</v>
+      </c>
+      <c r="CC5" t="s">
+        <v>170</v>
+      </c>
+      <c r="CD5" t="s">
+        <v>171</v>
+      </c>
+      <c r="CE5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CF5">
+        <v>9898989898</v>
+      </c>
+      <c r="CH5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N6" t="s">
+        <v>185</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>185</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+      <c r="X7" s="9">
+        <v>45043</v>
+      </c>
+      <c r="Y7">
+        <v>432</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>188</v>
+      </c>
+      <c r="N8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>189</v>
+      </c>
+      <c r="V9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7591CC6D-AE54-41C2-9DFC-DFE2C554B289}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{7BA0E2D2-3C09-483B-893F-0CBDB6B2EAC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6FDF44-3EC1-40BC-8A61-D5E9BA4325B7}">
+  <dimension ref="A1:AD12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>203</v>
+      </c>
+      <c r="T2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" t="s">
+        <v>209</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>210</v>
+      </c>
+      <c r="H4" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="N5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="S7">
+        <v>20</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="R8" t="s">
+        <v>203</v>
+      </c>
+      <c r="T8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="N9" t="s">
+        <v>213</v>
+      </c>
+      <c r="U9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>220</v>
+      </c>
+      <c r="W10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="X11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{76E0E862-F0BC-4EF3-8A41-706D0C808712}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{F4D254A0-A1CE-4E2F-AB99-92ABE05D84D7}"/>
+    <hyperlink ref="K5" r:id="rId3" xr:uid="{19CE02E2-1A12-4B0D-A5B5-9796FA3CEC43}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in CartPrice rule Code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{8B920716-312D-4BA3-89C3-26C846691877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34A31D3-D576-460F-9305-E4410BB91684}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="10275" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="10275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -788,6 +788,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,7 +1967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6FDF44-3EC1-40BC-8A61-D5E9BA4325B7}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Osprey Admin Helper, test case, testdata, Upsells
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20453A7E-D766-4F53-A51F-A72946978FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348DB1E7-BEC5-4A54-B1A7-EACC9F01CCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23040" windowHeight="12732" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="Pmanagement" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Upsells" sheetId="7" r:id="rId3"/>
     <sheet name="Category" sheetId="2" r:id="rId4"/>
     <sheet name="CartRulePrice" sheetId="3" r:id="rId5"/>
     <sheet name="CatalogPricerule" sheetId="4" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="270">
   <si>
     <t>DataSet</t>
   </si>
@@ -757,13 +757,91 @@
   </si>
   <si>
     <t>AETHER55</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>sukunta@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Azxcvbnmlkjh1@</t>
+  </si>
+  <si>
+    <t>TEST Product!</t>
+  </si>
+  <si>
+    <t>https://emea-preprod.hele.digital/</t>
+  </si>
+  <si>
+    <t>Dashboard / Magento Admin</t>
+  </si>
+  <si>
+    <t>promocontent</t>
+  </si>
+  <si>
+    <t>QA Testing on Promo Block Components-Content Changes</t>
+  </si>
+  <si>
+    <t>The page has been deleted.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/V_58eaD1NII</t>
+  </si>
+  <si>
+    <t>QA test for the hydrflask and promo content</t>
+  </si>
+  <si>
+    <t>#8fb8e3</t>
+  </si>
+  <si>
+    <t>Top Left</t>
+  </si>
+  <si>
+    <t>Qatestvalueprop</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#343434</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
+    <t>Valuepropbanner</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>valuepropcard2</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>valuepropcard3</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
+    <t>FlushMagento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +891,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303030"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -847,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -864,6 +954,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1151,62 +1244,62 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" customWidth="1"/>
-    <col min="6" max="6" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5546875" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.88671875" customWidth="1"/>
-    <col min="12" max="12" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.88671875" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.88671875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1352,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1365,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1335,17 +1428,17 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="33.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1482,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1506,7 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>178</v>
       </c>
@@ -1433,7 +1526,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>232</v>
       </c>
@@ -1453,7 +1546,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>233</v>
       </c>
@@ -1483,7 +1576,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>237</v>
       </c>
@@ -1503,7 +1596,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>238</v>
       </c>
@@ -1523,7 +1616,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>239</v>
       </c>
@@ -1545,7 +1638,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>240</v>
       </c>
@@ -1565,7 +1658,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>241</v>
       </c>
@@ -1585,7 +1678,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>242</v>
       </c>
@@ -1605,7 +1698,7 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1632,12 +1725,459 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8A686F-1F47-4C07-A6EF-DDDB500FE5C7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+    </row>
+    <row r="2" spans="1:36" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" s="14">
+        <v>23164</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="V3" s="11">
+        <v>25</v>
+      </c>
+      <c r="W3" s="11">
+        <v>27</v>
+      </c>
+      <c r="X3" s="11">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="11">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="11">
+        <v>35</v>
+      </c>
+      <c r="AB3" s="11">
+        <v>32</v>
+      </c>
+      <c r="AC3" s="11">
+        <v>23</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11">
+        <v>25</v>
+      </c>
+      <c r="W4" s="11">
+        <v>27</v>
+      </c>
+      <c r="X4" s="11">
+        <v>15</v>
+      </c>
+      <c r="Y4" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="11">
+        <v>30</v>
+      </c>
+      <c r="AA4" s="11">
+        <v>35</v>
+      </c>
+      <c r="AB4" s="11">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="11">
+        <v>23</v>
+      </c>
+      <c r="AD4" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11">
+        <v>12</v>
+      </c>
+      <c r="W5" s="11">
+        <v>32</v>
+      </c>
+      <c r="X5" s="11">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="11">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="11">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="11">
+        <v>20</v>
+      </c>
+      <c r="AB5" s="11">
+        <v>32</v>
+      </c>
+      <c r="AC5" s="11">
+        <v>21</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11">
+        <v>32</v>
+      </c>
+      <c r="W6" s="11">
+        <v>34</v>
+      </c>
+      <c r="X6" s="11">
+        <v>54</v>
+      </c>
+      <c r="Y6" s="11">
+        <v>21</v>
+      </c>
+      <c r="Z6" s="11">
+        <v>13</v>
+      </c>
+      <c r="AA6" s="11">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="11">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="11">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF7" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y7:Z7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="mailto:sukunta@helenoftroy.com" xr:uid="{4ACDCB13-C40B-45F2-BB42-3DEDF7E0CD23}"/>
+    <hyperlink ref="C2" r:id="rId2" display="mailto:Azxcvbnmlkjh1@" xr:uid="{959370FA-8B32-464D-8E18-B5255FD01B12}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{A534D69A-3F71-4EE7-AC39-08470280DEBF}"/>
+    <hyperlink ref="H2" r:id="rId4" xr:uid="{50FE86BF-1F45-4D10-8007-D1A36BF6F9E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1650,9 +2190,9 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +2230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1705,7 +2245,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1714,7 +2254,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1743,7 +2283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1767,9 +2307,9 @@
       <selection sqref="A1:DU9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2686,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2220,7 +2760,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -2234,7 +2774,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -2251,7 +2791,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2310,7 +2850,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -2327,7 +2867,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -2341,7 +2881,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2349,7 +2889,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:125" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2374,9 +2914,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2468,7 +3008,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2485,7 +3025,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -2508,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -2525,7 +3065,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2537,7 +3077,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -2557,7 +3097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -2577,7 +3117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>217</v>
       </c>
@@ -2588,7 +3128,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -2603,7 +3143,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -2611,7 +3151,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2619,7 +3159,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
Order Management Admin test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348DB1E7-BEC5-4A54-B1A7-EACC9F01CCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E027E46E-CD17-43A6-8E9C-83139161ADF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
     <sheet name="Pmanagement" sheetId="5" r:id="rId2"/>
     <sheet name="Upsells" sheetId="7" r:id="rId3"/>
-    <sheet name="Category" sheetId="2" r:id="rId4"/>
-    <sheet name="CartRulePrice" sheetId="3" r:id="rId5"/>
-    <sheet name="CatalogPricerule" sheetId="4" r:id="rId6"/>
+    <sheet name="Order_Management" sheetId="8" r:id="rId4"/>
+    <sheet name="Category" sheetId="2" r:id="rId5"/>
+    <sheet name="CartRulePrice" sheetId="3" r:id="rId6"/>
+    <sheet name="CatalogPricerule" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="297">
   <si>
     <t>DataSet</t>
   </si>
@@ -835,6 +836,87 @@
   </si>
   <si>
     <t>FlushMagento</t>
+  </si>
+  <si>
+    <t>dataSet</t>
+  </si>
+  <si>
+    <t>OrderDetails</t>
+  </si>
+  <si>
+    <t>InvoiceComments</t>
+  </si>
+  <si>
+    <t>ShipmentComments</t>
+  </si>
+  <si>
+    <t>CreditmemoComments</t>
+  </si>
+  <si>
+    <t>Phonenumber</t>
+  </si>
+  <si>
+    <t>gnarra@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>AnjSamgaS@6114!</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Creditmemo</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>Simple1,Simple2</t>
+  </si>
+  <si>
+    <t>'10/28</t>
+  </si>
+  <si>
+    <t>4242 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>OrderID</t>
+  </si>
+  <si>
+    <t>1000001468</t>
+  </si>
+  <si>
+    <t>BillingAddress</t>
+  </si>
+  <si>
+    <t>6 Walnut Valley Dr</t>
+  </si>
+  <si>
+    <t>Hot Springs Village</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>ShippingAddress</t>
+  </si>
+  <si>
+    <t>6333 Lookout Rd</t>
+  </si>
+  <si>
+    <t>Boulder</t>
+  </si>
+  <si>
+    <t>Colorado</t>
   </si>
 </sst>
 </file>
@@ -937,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -957,6 +1039,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1244,62 +1328,62 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.85546875" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.85546875" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.54296875" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.81640625" customWidth="1"/>
+    <col min="12" max="12" width="54.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.81640625" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1436,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1365,7 +1449,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1428,17 +1512,17 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="4" max="4" width="42.81640625" customWidth="1"/>
+    <col min="5" max="5" width="28.7265625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="12" max="12" width="33.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1566,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1506,7 +1590,7 @@
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>178</v>
       </c>
@@ -1526,7 +1610,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>232</v>
       </c>
@@ -1546,7 +1630,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>233</v>
       </c>
@@ -1576,7 +1660,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>237</v>
       </c>
@@ -1596,7 +1680,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>238</v>
       </c>
@@ -1616,7 +1700,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>239</v>
       </c>
@@ -1638,7 +1722,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>240</v>
       </c>
@@ -1658,7 +1742,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>241</v>
       </c>
@@ -1678,7 +1762,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>242</v>
       </c>
@@ -1698,7 +1782,7 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1727,19 +1811,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8A686F-1F47-4C07-A6EF-DDDB500FE5C7}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1839,7 +1923,7 @@
       <c r="AI1" s="10"/>
       <c r="AJ1" s="10"/>
     </row>
-    <row r="2" spans="1:36" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1891,7 +1975,7 @@
       <c r="AE2" s="11"/>
       <c r="AF2" s="11"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>251</v>
       </c>
@@ -1967,7 +2051,7 @@
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>263</v>
       </c>
@@ -2021,7 +2105,7 @@
       <c r="AE4" s="11"/>
       <c r="AF4" s="11"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>265</v>
       </c>
@@ -2075,7 +2159,7 @@
       <c r="AE5" s="11"/>
       <c r="AF5" s="11"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>267</v>
       </c>
@@ -2129,7 +2213,7 @@
       <c r="AE6" s="11"/>
       <c r="AF6" s="11"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>269</v>
       </c>
@@ -2183,6 +2267,223 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5881406-5AE1-41D6-A9E7-7BA759A04090}">
+  <dimension ref="A1:X6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="7"/>
+      <c r="P2" t="s">
+        <v>250</v>
+      </c>
+      <c r="X2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>282</v>
+      </c>
+      <c r="L3" t="s">
+        <v>283</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="N3">
+        <v>432</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="R3" t="s">
+        <v>173</v>
+      </c>
+      <c r="S3" t="s">
+        <v>171</v>
+      </c>
+      <c r="T3">
+        <v>6492</v>
+      </c>
+      <c r="U3">
+        <v>9898989898</v>
+      </c>
+      <c r="V3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>290</v>
+      </c>
+      <c r="S5" t="s">
+        <v>291</v>
+      </c>
+      <c r="T5">
+        <v>72211</v>
+      </c>
+      <c r="U5">
+        <v>9999999999</v>
+      </c>
+      <c r="W5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>294</v>
+      </c>
+      <c r="S6" t="s">
+        <v>295</v>
+      </c>
+      <c r="T6">
+        <v>80301</v>
+      </c>
+      <c r="U6">
+        <v>9999999999</v>
+      </c>
+      <c r="W6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4448D4CD-BB41-4F11-9A6F-316CFA3D3760}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1810791-6AFF-44EB-BA66-A2C45D322E0B}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -2190,9 +2491,9 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2546,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2254,7 +2555,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2283,7 +2584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2299,7 +2600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5005B9DD-FA95-4DB7-BA01-87E095E7225F}">
   <dimension ref="A1:DU9"/>
   <sheetViews>
@@ -2307,9 +2608,9 @@
       <selection sqref="A1:DU9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2760,7 +3061,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -2774,7 +3075,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -2791,7 +3092,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2850,7 +3151,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -2867,7 +3168,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -2881,7 +3182,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -2889,7 +3190,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:125" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:125" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2906,7 +3207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6FDF44-3EC1-40BC-8A61-D5E9BA4325B7}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
@@ -2914,9 +3215,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3008,7 +3309,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3025,7 +3326,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3048,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -3065,7 +3366,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3077,7 +3378,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -3097,7 +3398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -3117,7 +3418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>217</v>
       </c>
@@ -3128,7 +3429,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -3143,7 +3444,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -3151,7 +3452,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -3159,7 +3460,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>221</v>
       </c>

</xml_diff>

<commit_message>
Osprey admin helper, 2 test cases, test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
+++ b/src/test/resources/TestData/Osprey_Admin/GoldAdminTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E027E46E-CD17-43A6-8E9C-83139161ADF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ECF9A0-01A1-44B7-B369-EC04DD030B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20490" windowHeight="9855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="301">
   <si>
     <t>DataSet</t>
   </si>
@@ -917,6 +917,18 @@
   </si>
   <si>
     <t>Colorado</t>
+  </si>
+  <si>
+    <t>update Attribute</t>
+  </si>
+  <si>
+    <t>Test Attribute</t>
+  </si>
+  <si>
+    <t>Test Attribute 1</t>
+  </si>
+  <si>
+    <t>23164</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -1038,9 +1050,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1328,62 +1341,62 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.54296875" customWidth="1"/>
-    <col min="8" max="8" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.81640625" customWidth="1"/>
-    <col min="12" max="12" width="54.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="54.81640625" customWidth="1"/>
-    <col min="15" max="15" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.85546875" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="54.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="255.81640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="255.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1449,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1449,7 +1462,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1506,23 +1519,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F642833-FC82-405A-BB6A-7B473FBB8A4D}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
-    <col min="4" max="4" width="42.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="12" max="12" width="33.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1565,8 +1580,14 @@
       <c r="N1" s="10" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1581,7 +1602,9 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="11"/>
+      <c r="G2" s="19" t="s">
+        <v>300</v>
+      </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
@@ -1589,8 +1612,14 @@
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>298</v>
+      </c>
+      <c r="P2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>178</v>
       </c>
@@ -1610,7 +1639,7 @@
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>232</v>
       </c>
@@ -1630,7 +1659,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>233</v>
       </c>
@@ -1660,7 +1689,7 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>237</v>
       </c>
@@ -1680,7 +1709,7 @@
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>238</v>
       </c>
@@ -1700,7 +1729,7 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>239</v>
       </c>
@@ -1722,7 +1751,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>240</v>
       </c>
@@ -1742,7 +1771,7 @@
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>241</v>
       </c>
@@ -1762,7 +1791,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>242</v>
       </c>
@@ -1782,7 +1811,7 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1815,15 +1844,15 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1952,7 @@
       <c r="AI1" s="10"/>
       <c r="AJ1" s="10"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -1966,8 +1995,8 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
       <c r="AA2" s="11"/>
       <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>
@@ -1975,7 +2004,7 @@
       <c r="AE2" s="11"/>
       <c r="AF2" s="11"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>251</v>
       </c>
@@ -2051,7 +2080,7 @@
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>263</v>
       </c>
@@ -2105,7 +2134,7 @@
       <c r="AE4" s="11"/>
       <c r="AF4" s="11"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>265</v>
       </c>
@@ -2159,7 +2188,7 @@
       <c r="AE5" s="11"/>
       <c r="AF5" s="11"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>267</v>
       </c>
@@ -2213,7 +2242,7 @@
       <c r="AE6" s="11"/>
       <c r="AF6" s="11"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>269</v>
       </c>
@@ -2240,8 +2269,8 @@
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="11"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
       <c r="AC7" s="11"/>
@@ -2270,13 +2299,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5881406-5AE1-41D6-A9E7-7BA759A04090}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>270</v>
       </c>
@@ -2350,7 +2379,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2361,10 +2390,10 @@
         <v>277</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>279</v>
       </c>
       <c r="H2" s="7" t="s">
@@ -2380,11 +2409,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>281</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="2"/>
@@ -2393,7 +2422,7 @@
       <c r="I3" t="s">
         <v>170</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="16" t="s">
         <v>15</v>
       </c>
       <c r="K3" t="s">
@@ -2408,7 +2437,7 @@
       <c r="N3">
         <v>432</v>
       </c>
-      <c r="O3" s="18" t="s">
+      <c r="O3" s="17" t="s">
         <v>285</v>
       </c>
       <c r="R3" t="s">
@@ -2427,7 +2456,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>287</v>
       </c>
@@ -2435,7 +2464,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -2455,7 +2484,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -2491,9 +2520,9 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2531,7 +2560,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2546,7 +2575,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2555,7 +2584,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2584,7 +2613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2608,9 +2637,9 @@
       <selection sqref="A1:DU9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +3016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3061,7 +3090,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3075,7 +3104,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -3092,7 +3121,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3151,7 +3180,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -3168,7 +3197,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -3182,7 +3211,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -3190,7 +3219,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:125" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:125" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -3215,9 +3244,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3309,7 +3338,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3326,7 +3355,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3349,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
@@ -3366,7 +3395,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3378,7 +3407,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -3398,7 +3427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -3418,7 +3447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>217</v>
       </c>
@@ -3429,7 +3458,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>174</v>
       </c>
@@ -3444,7 +3473,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>220</v>
       </c>
@@ -3452,7 +3481,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -3460,7 +3489,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>221</v>
       </c>

</xml_diff>